<commit_message>
translate diagrams columns to english
</commit_message>
<xml_diff>
--- a/pp/gantt/PowerEnJoyGantt.xlsx
+++ b/pp/gantt/PowerEnJoyGantt.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19155" windowHeight="9030"/>
   </bookViews>
   <sheets>
-    <sheet name="RASD" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -26,36 +26,45 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
-    <t>N. attività</t>
-  </si>
-  <si>
-    <t>Nome attività</t>
-  </si>
-  <si>
-    <t>Durata</t>
-  </si>
-  <si>
-    <t>Data inizio</t>
-  </si>
-  <si>
-    <t>Data fine</t>
-  </si>
-  <si>
-    <t>Dipendenza</t>
-  </si>
-  <si>
-    <t>Risorsa</t>
-  </si>
-  <si>
-    <t>Livello struttura</t>
+    <t>Task #</t>
+  </si>
+  <si>
+    <t>Task Name</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>Finish Date</t>
+  </si>
+  <si>
+    <t>Dependency</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Outline Level</t>
+  </si>
+  <si>
+    <t>Task Notes</t>
   </si>
   <si>
     <t>RASD</t>
   </si>
   <si>
+    <t>Davide, Mario, Moreno</t>
+  </si>
+  <si>
     <t>Meetings with client</t>
   </si>
   <si>
+    <t>All the resources will be present at the meeting</t>
+  </si>
+  <si>
     <t>Identification of goals and stakeholders</t>
   </si>
   <si>
@@ -65,6 +74,9 @@
     <t>Modelization of the World and the Machine</t>
   </si>
   <si>
+    <t>This part requires discussion and cooperation, hence it will be assigned to all the resources</t>
+  </si>
+  <si>
     <t>Identification of domain assumptions</t>
   </si>
   <si>
@@ -77,15 +89,27 @@
     <t>Writing scenarios</t>
   </si>
   <si>
+    <t>Davide, Moreno</t>
+  </si>
+  <si>
     <t>Identification of use cases</t>
   </si>
   <si>
+    <t>Moreno</t>
+  </si>
+  <si>
     <t>Identification of needed data</t>
   </si>
   <si>
+    <t>Davide</t>
+  </si>
+  <si>
     <t>Alloy model draft</t>
   </si>
   <si>
+    <t>Mario</t>
+  </si>
+  <si>
     <t>In progress meeting with client</t>
   </si>
   <si>
@@ -93,49 +117,25 @@
   </si>
   <si>
     <t>Requirements refinement</t>
-  </si>
-  <si>
-    <t>Data model refinement</t>
-  </si>
-  <si>
-    <t>Sequence diagrams for use cases</t>
-  </si>
-  <si>
-    <t>Alloy modelization</t>
-  </si>
-  <si>
-    <t>Davide, Mario, Moreno</t>
-  </si>
-  <si>
-    <t>Davide</t>
-  </si>
-  <si>
-    <t>Mario, Davide</t>
-  </si>
-  <si>
-    <t>Mario</t>
-  </si>
-  <si>
-    <t>Moreno</t>
-  </si>
-  <si>
-    <t>Commento</t>
-  </si>
-  <si>
-    <t>Davide will start working on this activity in date 05/11/2016</t>
-  </si>
-  <si>
-    <t>Davide, Moreno</t>
-  </si>
-  <si>
-    <t>All the resources will be present at the meeting</t>
   </si>
   <si>
     <t>The requirements will be updated based on updates made 
 in other parts of the document, during its developement</t>
   </si>
   <si>
-    <t>This part requires discussion and cooperation, hence it will be assigned to all the resources</t>
+    <t>Data model refinement</t>
+  </si>
+  <si>
+    <t>Sequence diagrams for use cases</t>
+  </si>
+  <si>
+    <t>Alloy modelization</t>
+  </si>
+  <si>
+    <t>Mario, Davide</t>
+  </si>
+  <si>
+    <t>Davide will start working on this activity in date 05/11/2016</t>
   </si>
 </sst>
 </file>
@@ -180,17 +180,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -206,7 +205,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -502,31 +501,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.42578125" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="21" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" customWidth="1"/>
-    <col min="16" max="20" width="20" customWidth="1"/>
-    <col min="21" max="21" width="19.7109375" customWidth="1"/>
-    <col min="22" max="22" width="20" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" customWidth="1"/>
+    <col min="16" max="20" width="19.7109375" customWidth="1"/>
+    <col min="21" max="21" width="21.7109375" customWidth="1"/>
+    <col min="22" max="22" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -540,7 +539,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -576,10 +575,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE(NETWORKDAYS(F2,G2),"g")</f>
@@ -602,13 +601,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E19" si="0">CONCATENATE(NETWORKDAYS(F3,G3),"g")</f>
@@ -631,10 +630,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" si="0"/>
@@ -657,10 +656,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E5" t="str">
         <f>CONCATENATE(NETWORKDAYS(F5,G5),"g")</f>
@@ -683,13 +682,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="0"/>
@@ -712,10 +711,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="0"/>
@@ -736,10 +735,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="0"/>
@@ -760,10 +759,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="0"/>
@@ -784,10 +783,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="0"/>
@@ -808,10 +807,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="0"/>
@@ -835,10 +834,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="0"/>
@@ -859,10 +858,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="0"/>
@@ -883,13 +882,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="0"/>
@@ -910,10 +909,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="0"/>
@@ -934,13 +933,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="0"/>
@@ -961,10 +960,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="0"/>
@@ -985,10 +984,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="0"/>
@@ -1009,13 +1008,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="0"/>
@@ -1030,9 +1029,6 @@
       <c r="I19">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>